<commit_message>
Ran cs_scrape and adjusted code due to xsxl output
</commit_message>
<xml_diff>
--- a/Scholarships Research.xlsx
+++ b/Scholarships Research.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://westernsydneyedu.sharepoint.com/sites/ScholarshipsOperationsGroup/Shared Documents/Git/Scholarships/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{891E6A58-1632-490F-A8B6-5FDA491183CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B1C5751D-AA5E-410A-9380-36C08CD9C92B}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{891E6A58-1632-490F-A8B6-5FDA491183CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{59F1490C-7DC7-475D-BDB1-6E1422CDF732}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1CF3EDB6-384E-4233-A2F8-DD99A8F9DE7B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1CF3EDB6-384E-4233-A2F8-DD99A8F9DE7B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <externalReference r:id="rId2"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$176</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$G$1:$G$176</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1315,8 +1315,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5773BD61-A8F4-4ACA-BB03-11DEBD312DAE}">
   <dimension ref="A1:I176"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="A164" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6129,13 +6129,33 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H176" xr:uid="{5773BD61-A8F4-4ACA-BB03-11DEBD312DAE}"/>
+  <autoFilter ref="G1:G176" xr:uid="{5773BD61-A8F4-4ACA-BB03-11DEBD312DAE}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="91d47d42-378c-4240-adf1-50612b639f36" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="514dc54e-a510-4ebc-96a4-7a373c84d576">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A1B59F058DD61F4CBF5D961017DC0A45" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3843482ad259dd7cf47d53181de3a479">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="514dc54e-a510-4ebc-96a4-7a373c84d576" xmlns:ns3="91d47d42-378c-4240-adf1-50612b639f36" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c2a99e4d2b0f67119e90f9a433f5d6db" ns2:_="" ns3:_="">
     <xsd:import namespace="514dc54e-a510-4ebc-96a4-7a373c84d576"/>
@@ -6384,27 +6404,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{931EF037-3A45-438F-8EFF-A0227E591D57}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="91d47d42-378c-4240-adf1-50612b639f36"/>
+    <ds:schemaRef ds:uri="514dc54e-a510-4ebc-96a4-7a373c84d576"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="91d47d42-378c-4240-adf1-50612b639f36" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="514dc54e-a510-4ebc-96a4-7a373c84d576">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2939E453-00EA-486F-995B-7D4644B61C8A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{873E4114-4F26-4870-B334-33A2DDABEBD5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6421,23 +6440,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2939E453-00EA-486F-995B-7D4644B61C8A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{931EF037-3A45-438F-8EFF-A0227E591D57}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="91d47d42-378c-4240-adf1-50612b639f36"/>
-    <ds:schemaRef ds:uri="514dc54e-a510-4ebc-96a4-7a373c84d576"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
script for usyd urls & pickled
</commit_message>
<xml_diff>
--- a/Scholarships Research.xlsx
+++ b/Scholarships Research.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{BC4AE9FA-0CB4-4CF0-8D39-57A9F105CFA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{712ABEEC-36FC-47A3-BE68-20EE75D1D2EC}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1CF3EDB6-384E-4233-A2F8-DD99A8F9DE7B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1CF3EDB6-384E-4233-A2F8-DD99A8F9DE7B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19766,6 +19766,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="91d47d42-378c-4240-adf1-50612b639f36" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="514dc54e-a510-4ebc-96a4-7a373c84d576">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A1B59F058DD61F4CBF5D961017DC0A45" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3843482ad259dd7cf47d53181de3a479">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="514dc54e-a510-4ebc-96a4-7a373c84d576" xmlns:ns3="91d47d42-378c-4240-adf1-50612b639f36" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c2a99e4d2b0f67119e90f9a433f5d6db" ns2:_="" ns3:_="">
     <xsd:import namespace="514dc54e-a510-4ebc-96a4-7a373c84d576"/>
@@ -20014,27 +20034,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{931EF037-3A45-438F-8EFF-A0227E591D57}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="91d47d42-378c-4240-adf1-50612b639f36"/>
+    <ds:schemaRef ds:uri="514dc54e-a510-4ebc-96a4-7a373c84d576"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="91d47d42-378c-4240-adf1-50612b639f36" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="514dc54e-a510-4ebc-96a4-7a373c84d576">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2939E453-00EA-486F-995B-7D4644B61C8A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{873E4114-4F26-4870-B334-33A2DDABEBD5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -20051,23 +20070,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2939E453-00EA-486F-995B-7D4644B61C8A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{931EF037-3A45-438F-8EFF-A0227E591D57}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="91d47d42-378c-4240-adf1-50612b639f36"/>
-    <ds:schemaRef ds:uri="514dc54e-a510-4ebc-96a4-7a373c84d576"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Changed approach to USYD, scraped old code
</commit_message>
<xml_diff>
--- a/Scholarships Research.xlsx
+++ b/Scholarships Research.xlsx
@@ -19766,26 +19766,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="91d47d42-378c-4240-adf1-50612b639f36" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="514dc54e-a510-4ebc-96a4-7a373c84d576">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A1B59F058DD61F4CBF5D961017DC0A45" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3843482ad259dd7cf47d53181de3a479">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="514dc54e-a510-4ebc-96a4-7a373c84d576" xmlns:ns3="91d47d42-378c-4240-adf1-50612b639f36" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c2a99e4d2b0f67119e90f9a433f5d6db" ns2:_="" ns3:_="">
     <xsd:import namespace="514dc54e-a510-4ebc-96a4-7a373c84d576"/>
@@ -20034,26 +20014,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{931EF037-3A45-438F-8EFF-A0227E591D57}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="91d47d42-378c-4240-adf1-50612b639f36"/>
-    <ds:schemaRef ds:uri="514dc54e-a510-4ebc-96a4-7a373c84d576"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2939E453-00EA-486F-995B-7D4644B61C8A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="91d47d42-378c-4240-adf1-50612b639f36" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="514dc54e-a510-4ebc-96a4-7a373c84d576">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{873E4114-4F26-4870-B334-33A2DDABEBD5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -20070,4 +20051,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2939E453-00EA-486F-995B-7D4644B61C8A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{931EF037-3A45-438F-8EFF-A0227E591D57}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="91d47d42-378c-4240-adf1-50612b639f36"/>
+    <ds:schemaRef ds:uri="514dc54e-a510-4ebc-96a4-7a373c84d576"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
started manual adjustment of USYD
</commit_message>
<xml_diff>
--- a/Scholarships Research.xlsx
+++ b/Scholarships Research.xlsx
@@ -3803,7 +3803,7 @@
   <dimension ref="A1:I531"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B336" sqref="B336"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19766,6 +19766,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="91d47d42-378c-4240-adf1-50612b639f36" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="514dc54e-a510-4ebc-96a4-7a373c84d576">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A1B59F058DD61F4CBF5D961017DC0A45" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3843482ad259dd7cf47d53181de3a479">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="514dc54e-a510-4ebc-96a4-7a373c84d576" xmlns:ns3="91d47d42-378c-4240-adf1-50612b639f36" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c2a99e4d2b0f67119e90f9a433f5d6db" ns2:_="" ns3:_="">
     <xsd:import namespace="514dc54e-a510-4ebc-96a4-7a373c84d576"/>
@@ -20014,27 +20034,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{931EF037-3A45-438F-8EFF-A0227E591D57}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="91d47d42-378c-4240-adf1-50612b639f36"/>
+    <ds:schemaRef ds:uri="514dc54e-a510-4ebc-96a4-7a373c84d576"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="91d47d42-378c-4240-adf1-50612b639f36" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="514dc54e-a510-4ebc-96a4-7a373c84d576">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2939E453-00EA-486F-995B-7D4644B61C8A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{873E4114-4F26-4870-B334-33A2DDABEBD5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -20051,23 +20070,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2939E453-00EA-486F-995B-7D4644B61C8A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{931EF037-3A45-438F-8EFF-A0227E591D57}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="91d47d42-378c-4240-adf1-50612b639f36"/>
-    <ds:schemaRef ds:uri="514dc54e-a510-4ebc-96a4-7a373c84d576"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
last commit did not work
</commit_message>
<xml_diff>
--- a/Scholarships Research.xlsx
+++ b/Scholarships Research.xlsx
@@ -18967,6 +18967,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="91d47d42-378c-4240-adf1-50612b639f36" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="514dc54e-a510-4ebc-96a4-7a373c84d576">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A1B59F058DD61F4CBF5D961017DC0A45" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3843482ad259dd7cf47d53181de3a479">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="514dc54e-a510-4ebc-96a4-7a373c84d576" xmlns:ns3="91d47d42-378c-4240-adf1-50612b639f36" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c2a99e4d2b0f67119e90f9a433f5d6db" ns2:_="" ns3:_="">
     <xsd:import namespace="514dc54e-a510-4ebc-96a4-7a373c84d576"/>
@@ -19215,27 +19235,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{931EF037-3A45-438F-8EFF-A0227E591D57}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="91d47d42-378c-4240-adf1-50612b639f36"/>
+    <ds:schemaRef ds:uri="514dc54e-a510-4ebc-96a4-7a373c84d576"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="91d47d42-378c-4240-adf1-50612b639f36" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="514dc54e-a510-4ebc-96a4-7a373c84d576">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2939E453-00EA-486F-995B-7D4644B61C8A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{873E4114-4F26-4870-B334-33A2DDABEBD5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -19252,23 +19271,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2939E453-00EA-486F-995B-7D4644B61C8A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{931EF037-3A45-438F-8EFF-A0227E591D57}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="91d47d42-378c-4240-adf1-50612b639f36"/>
-    <ds:schemaRef ds:uri="514dc54e-a510-4ebc-96a4-7a373c84d576"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Manual work for USYD (ick)
</commit_message>
<xml_diff>
--- a/Scholarships Research.xlsx
+++ b/Scholarships Research.xlsx
@@ -3513,7 +3513,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5773BD61-A8F4-4ACA-BB03-11DEBD312DAE}">
   <dimension ref="A1:I514"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A280" workbookViewId="0">
       <selection activeCell="C387" sqref="C387"/>
     </sheetView>
   </sheetViews>
@@ -18967,26 +18967,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="91d47d42-378c-4240-adf1-50612b639f36" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="514dc54e-a510-4ebc-96a4-7a373c84d576">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A1B59F058DD61F4CBF5D961017DC0A45" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3843482ad259dd7cf47d53181de3a479">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="514dc54e-a510-4ebc-96a4-7a373c84d576" xmlns:ns3="91d47d42-378c-4240-adf1-50612b639f36" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c2a99e4d2b0f67119e90f9a433f5d6db" ns2:_="" ns3:_="">
     <xsd:import namespace="514dc54e-a510-4ebc-96a4-7a373c84d576"/>
@@ -19235,26 +19215,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{931EF037-3A45-438F-8EFF-A0227E591D57}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="91d47d42-378c-4240-adf1-50612b639f36"/>
-    <ds:schemaRef ds:uri="514dc54e-a510-4ebc-96a4-7a373c84d576"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2939E453-00EA-486F-995B-7D4644B61C8A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="91d47d42-378c-4240-adf1-50612b639f36" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="514dc54e-a510-4ebc-96a4-7a373c84d576">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{873E4114-4F26-4870-B334-33A2DDABEBD5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -19271,4 +19252,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2939E453-00EA-486F-995B-7D4644B61C8A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{931EF037-3A45-438F-8EFF-A0227E591D57}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="91d47d42-378c-4240-adf1-50612b639f36"/>
+    <ds:schemaRef ds:uri="514dc54e-a510-4ebc-96a4-7a373c84d576"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
made changes in USYD file
</commit_message>
<xml_diff>
--- a/Scholarships Research.xlsx
+++ b/Scholarships Research.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="327" documentId="13_ncr:1_{BC4AE9FA-0CB4-4CF0-8D39-57A9F105CFA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F6ACF66A-E258-4133-9385-0065CDCF93BA}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1CF3EDB6-384E-4233-A2F8-DD99A8F9DE7B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1CF3EDB6-384E-4233-A2F8-DD99A8F9DE7B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3513,7 +3513,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5773BD61-A8F4-4ACA-BB03-11DEBD312DAE}">
   <dimension ref="A1:I514"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A280" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C387" sqref="C387"/>
     </sheetView>
   </sheetViews>

</xml_diff>